<commit_message>
nameless commits and updated gitignore
</commit_message>
<xml_diff>
--- a/data/test_raw_data.xlsx
+++ b/data/test_raw_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rlm/Documents/openProjects/Python-Projects/Data-Transformation-and-Cleaning-Automation-Tool/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A16F2C4A-35CD-C74B-9F0D-03E34DB891DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE145786-9BCA-8040-AABE-C0EFE700778F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="21000" xr2:uid="{58CB86B2-7F0D-F046-85E2-7871710B5CC3}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="16800" windowHeight="21000" xr2:uid="{58CB86B2-7F0D-F046-85E2-7871710B5CC3}"/>
   </bookViews>
   <sheets>
     <sheet name="test_raw_data" sheetId="1" r:id="rId1"/>
@@ -3852,7 +3852,7 @@
   <dimension ref="A1:J1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>